<commit_message>
metadata and cellranger scripts added
</commit_message>
<xml_diff>
--- a/multiomics/data/multiomics_brain_sample_metadata.xlsx
+++ b/multiomics/data/multiomics_brain_sample_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvarani.masarapu/Documents/GitHub/NASA-RR3_Brain/multiomics/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yuvarani.masarapu/Documents/GitHub/NASA_RR3_Brain/multiomics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B76D8C4-F40B-F846-870A-729225FBEDE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71FBC705-0EDD-5B47-BB71-84DE6A01113C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15360" yWindow="500" windowWidth="15360" windowHeight="17100" xr2:uid="{A2FA3A16-0CBC-3E4E-B38D-CE215FCCF730}"/>
+    <workbookView xWindow="15360" yWindow="500" windowWidth="15360" windowHeight="17000" xr2:uid="{A2FA3A16-0CBC-3E4E-B38D-CE215FCCF730}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,35 +44,35 @@
     <t>Organ</t>
   </si>
   <si>
-    <t>Mice_ID</t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
     <t>Brain</t>
   </si>
   <si>
-    <t>CF1_B</t>
-  </si>
-  <si>
-    <t>CF2_B</t>
-  </si>
-  <si>
-    <t>CF7_B</t>
-  </si>
-  <si>
-    <t>CG8_B</t>
-  </si>
-  <si>
-    <t>CG9_B</t>
+    <t>Mice_id</t>
+  </si>
+  <si>
+    <t>F1</t>
+  </si>
+  <si>
+    <t>F2</t>
+  </si>
+  <si>
+    <t>F3</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -87,12 +87,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,9 +109,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -137,7 +130,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -425,7 +418,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -433,95 +426,83 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{047927F2-CAF4-F242-AC64-28FDCA174698}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
         <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
         <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>